<commit_message>
Agrego casos de prueba en matriz
</commit_message>
<xml_diff>
--- a/casos_de_prueba/matriz_pruebas.xlsx
+++ b/casos_de_prueba/matriz_pruebas.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ProyectoFinal\ProyectoFinal-Nerea\casos_de_prueba\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB83ED-4D5B-4FC7-B758-72D04BFB38B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="203">
   <si>
     <t>Nombre del Proyecto:</t>
   </si>
@@ -152,52 +161,538 @@
   </si>
   <si>
     <t>CP30</t>
+  </si>
+  <si>
+    <t>Registro exitoso con datos válidos</t>
+  </si>
+  <si>
+    <t>Validar que el sistema permite registrar un usuario con username y email válido.</t>
+  </si>
+  <si>
+    <t>Acceso a la app; pantalla Crear cuenta nueva</t>
+  </si>
+  <si>
+    <t>Email: qa_user31@hotmail.com ; Contraseña: testing.26</t>
+  </si>
+  <si>
+    <t>1)Completar email válido. 2)Siguiente.3)Completar con código enviado por mail.4) Completar nombre y contraseña.5) Completar preguntas de seguridad</t>
+  </si>
+  <si>
+    <t>Usuario creado correctamente</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Registro con email inválido</t>
+  </si>
+  <si>
+    <t>Error por email incorrecto</t>
+  </si>
+  <si>
+    <t>Email: qa_user31@hotmail</t>
+  </si>
+  <si>
+    <t>1)Completar email inválido. 2)Siguiente</t>
+  </si>
+  <si>
+    <t>Muestra Error</t>
+  </si>
+  <si>
+    <t>El sistema bloquea el botón "siguiente"</t>
+  </si>
+  <si>
+    <t>Registro con contraseña corta</t>
+  </si>
+  <si>
+    <t>Error por contraseña &lt;6 caracteres</t>
+  </si>
+  <si>
+    <t>nombre: qa_user31@hotmail.com ; Contraseña:12345</t>
+  </si>
+  <si>
+    <t>1)Completar email válido. 2)Siguiente3)completar codigo enviado por mail.4)completar nombre y contraseña CORTA</t>
+  </si>
+  <si>
+    <t>Muestra cartel de contraseña corta</t>
+  </si>
+  <si>
+    <t>Registro con contraseña larga</t>
+  </si>
+  <si>
+    <t>Validar contraseña larga</t>
+  </si>
+  <si>
+    <t>nombre: qa_user31 ; Contraseña:testing.268888888888</t>
+  </si>
+  <si>
+    <t>1)Completar email válido. 2)Siguiente3)completar codigo enviado por mail.4)completar nombre y contraseña LARGA</t>
+  </si>
+  <si>
+    <t>El sistema permite presionar botón "siguiente"</t>
+  </si>
+  <si>
+    <t>Email duplicado</t>
+  </si>
+  <si>
+    <t>Validar email ya registrado</t>
+  </si>
+  <si>
+    <t>Email: qa_user31@hotmail.com ; Contraseña:testing.268888888889</t>
+  </si>
+  <si>
+    <t>1)Completar email YA REGISTRADO. 2)Siguiente3)completar codigo enviado por mail.4)completar nombre y contraseña LARGA</t>
+  </si>
+  <si>
+    <t>Mensaje “email ya registrado”</t>
+  </si>
+  <si>
+    <t>Campo Email vacío</t>
+  </si>
+  <si>
+    <t>Error por campo email vacío</t>
+  </si>
+  <si>
+    <t>Email: VACIO</t>
+  </si>
+  <si>
+    <t>1)Email VACIO.2)Siguiente</t>
+  </si>
+  <si>
+    <t>Registro con email sin @</t>
+  </si>
+  <si>
+    <t>Error por email sin @</t>
+  </si>
+  <si>
+    <t>Email: qa_user31hotmail.com</t>
+  </si>
+  <si>
+    <t>1)Completar email sin @. 2)Siguiente</t>
+  </si>
+  <si>
+    <t>Registro con contraseña sin números</t>
+  </si>
+  <si>
+    <t>Error por contraseña sin números</t>
+  </si>
+  <si>
+    <t>Email:qa_user31@hotmail.com ; Contraseña: testing.test</t>
+  </si>
+  <si>
+    <t>1)Completar email válido. 2)Siguiente3)completar codigo enviado por mail.4)completar nombre y contraseña SIN NÚMEROS</t>
+  </si>
+  <si>
+    <t>Muestra cartel de ¨La contraseña debe tener números¨</t>
+  </si>
+  <si>
+    <t>El sistema permite contraseña y pasa a próximo paso</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Login correcto</t>
+  </si>
+  <si>
+    <t>Validar acceso con credenciales válidas</t>
+  </si>
+  <si>
+    <t>Acceso a la app; pantalla Iniciar Sesión</t>
+  </si>
+  <si>
+    <t>Usuario: qa_user31 ; Contraseña: testing.26</t>
+  </si>
+  <si>
+    <t>1)Completar usuario y contraseña válidas.2)apretar iniciar sesión</t>
+  </si>
+  <si>
+    <t>Acceso a pantalla principal</t>
+  </si>
+  <si>
+    <t>Contraseña incorrecta</t>
+  </si>
+  <si>
+    <t>Error por contraseña incorrecta</t>
+  </si>
+  <si>
+    <t>Usuario: qa_user31 ; Contraseña: testing.30</t>
+  </si>
+  <si>
+    <t>1)Completar usuario válido y contraseña inválidas.2)apretar iniciar sesión</t>
+  </si>
+  <si>
+    <t>Muestra mensaje de error</t>
+  </si>
+  <si>
+    <t>Email no registrado</t>
+  </si>
+  <si>
+    <t>Validar email no registrado</t>
+  </si>
+  <si>
+    <t>Acceso a la app; opción Inicia sesión</t>
+  </si>
+  <si>
+    <t>Email:qa.user98@hotmail.com ; Contraseña: testing.26</t>
+  </si>
+  <si>
+    <t>1)completar con email no registrado y contraseña válida;Iniciar sesión</t>
+  </si>
+  <si>
+    <t>No se puede acceder a cuenta</t>
+  </si>
+  <si>
+    <t>Campo de contraseña vacío</t>
+  </si>
+  <si>
+    <t>Validar campo obligatorio de login</t>
+  </si>
+  <si>
+    <t>Email:qa_user31@hotmail.com ; Contraseña: VACIO</t>
+  </si>
+  <si>
+    <t>1)completar con email válido y contraseña VACIO;Iniciar sesión</t>
+  </si>
+  <si>
+    <t>Muestra mensaje de "completar campo"</t>
+  </si>
+  <si>
+    <t>Cerrar sesión</t>
+  </si>
+  <si>
+    <t>Validar cierre de sesión exitoso</t>
+  </si>
+  <si>
+    <t>Sesión iniciada</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1)Ir a perfil.2)apretar las 3 lineas.4)cerrar sesión</t>
+  </si>
+  <si>
+    <t>Dirige a página de Login</t>
+  </si>
+  <si>
+    <t>Recuperar contraseña válido</t>
+  </si>
+  <si>
+    <t>Validar recuperación con email válido</t>
+  </si>
+  <si>
+    <t>Email registrado</t>
+  </si>
+  <si>
+    <t>Email:qa_user31@hotmail.com</t>
+  </si>
+  <si>
+    <t>1)Ingresar a login.2)Olvidé contraseña.3)Enviar</t>
+  </si>
+  <si>
+    <t>Se envia mail con link de recuperación</t>
+  </si>
+  <si>
+    <t>Ingresar más de 3 intentos fallidos de contraseña</t>
+  </si>
+  <si>
+    <t>Error por intentos fallidos</t>
+  </si>
+  <si>
+    <t>Ingresar Contraseña inválida: asdfghjk</t>
+  </si>
+  <si>
+    <t>1)Completar usuario y contraseña inválida</t>
+  </si>
+  <si>
+    <t>Se bloquea cuenta</t>
+  </si>
+  <si>
+    <t>El sistema permite seguir intentando</t>
+  </si>
+  <si>
+    <t>Comportamiento inconsistente al abrir publicaciones</t>
+  </si>
+  <si>
+    <t>Error al cargar publicaciones</t>
+  </si>
+  <si>
+    <t>Ingresar al perfil</t>
+  </si>
+  <si>
+    <t>1)Ingresar al feed.2)Seleccionar la primera publicación.3) Intentar mover la pantalla hacia arriba.4)Repetir con la publicación más reciente.</t>
+  </si>
+  <si>
+    <t>Se debe poder mover la pantalla de manera consistente</t>
+  </si>
+  <si>
+    <t>Al mover la pantalla, el comportamiento es inconsistente y algunas imágenes se cortan</t>
+  </si>
+  <si>
+    <t>Publicar foto nueva</t>
+  </si>
+  <si>
+    <t>Validar publicación con imagen</t>
+  </si>
+  <si>
+    <t>1)Presionar "+" en el inicio.2)Seleccionar foto y escribir descripción.3)Compartir</t>
+  </si>
+  <si>
+    <t>Foto visible en feed</t>
+  </si>
+  <si>
+    <t>Publicar foto sin descripción</t>
+  </si>
+  <si>
+    <t>Validar publicación sin descripción</t>
+  </si>
+  <si>
+    <t>1)Presionar "+" en el inicio.2)Seleccionar foto y dejar descripción Vacio.3)Compartir</t>
+  </si>
+  <si>
+    <t>Publicación exitosa</t>
+  </si>
+  <si>
+    <t>Editar descripción de publicación</t>
+  </si>
+  <si>
+    <t>Validar edición después de publicar</t>
+  </si>
+  <si>
+    <t>Tener publicada una foto</t>
+  </si>
+  <si>
+    <t>1)Presionar la foto.2)Presionar los 3 puntos.3)Editar.4)Editar publicación.5)Guardar</t>
+  </si>
+  <si>
+    <t>Guarda cambios correctamente</t>
+  </si>
+  <si>
+    <t>Publicar foto y activar modo avión antes de confirmar</t>
+  </si>
+  <si>
+    <t>Validar cancelación de posteo</t>
+  </si>
+  <si>
+    <t>Poner el celular en "modo avión"</t>
+  </si>
+  <si>
+    <t>1)Presionar "+" en el inicio.2)Seleccionar foto y escribir descripción.3)Poner celular en "modo avión".4)Compartir</t>
+  </si>
+  <si>
+    <t>Cancela el posteo de foto</t>
+  </si>
+  <si>
+    <t>No se cancela posteo</t>
+  </si>
+  <si>
+    <t>Dar like</t>
+  </si>
+  <si>
+    <t>Validar aumento de contador</t>
+  </si>
+  <si>
+    <t>Ingresar a perfil de usuario; seleccionar una foto</t>
+  </si>
+  <si>
+    <t>Click en "Me gusta"</t>
+  </si>
+  <si>
+    <t>Contador aumente +1</t>
+  </si>
+  <si>
+    <t>Contador aumenta +1</t>
+  </si>
+  <si>
+    <t>Quitar like</t>
+  </si>
+  <si>
+    <t>Validar disminución contador</t>
+  </si>
+  <si>
+    <t>Like previo</t>
+  </si>
+  <si>
+    <t>Contador diminuya -1</t>
+  </si>
+  <si>
+    <t>Contador diminuye -1</t>
+  </si>
+  <si>
+    <t>Like múltiple</t>
+  </si>
+  <si>
+    <t>Validar solo 1 me gusta</t>
+  </si>
+  <si>
+    <t>Click varias veces en "Me gusta"</t>
+  </si>
+  <si>
+    <t>Solo se cuenta 1 me gusta</t>
+  </si>
+  <si>
+    <t>Persistencia de like</t>
+  </si>
+  <si>
+    <t>Validar persistencia tras recarga</t>
+  </si>
+  <si>
+    <t>Recargar app</t>
+  </si>
+  <si>
+    <t>Like persiste</t>
+  </si>
+  <si>
+    <t>Comentario válido</t>
+  </si>
+  <si>
+    <t>Validar publicación de comentario</t>
+  </si>
+  <si>
+    <t>Seleccionar una publicación</t>
+  </si>
+  <si>
+    <t>1)Seleccionar publicación.2)Escribir comentario.3)Publicar</t>
+  </si>
+  <si>
+    <t>Se publica correctamente</t>
+  </si>
+  <si>
+    <t>Comentario vacío</t>
+  </si>
+  <si>
+    <t>Error por campo vacío</t>
+  </si>
+  <si>
+    <t>Dejar el campo "Añade un comentario" VACIO</t>
+  </si>
+  <si>
+    <t>Enviar comentario vacío</t>
+  </si>
+  <si>
+    <t>El sistema no permite publicar</t>
+  </si>
+  <si>
+    <t>Eliminar comentario propio</t>
+  </si>
+  <si>
+    <t>Validar eliminación comentario propio</t>
+  </si>
+  <si>
+    <t>Comentario publicado</t>
+  </si>
+  <si>
+    <t>Eliminar comentario publicado</t>
+  </si>
+  <si>
+    <t>Se elimina correctamente</t>
+  </si>
+  <si>
+    <t>Seguir usuario</t>
+  </si>
+  <si>
+    <t>Validar seguimiento exitoso</t>
+  </si>
+  <si>
+    <t>Acceder al perfil del usuario</t>
+  </si>
+  <si>
+    <t>1)Ingresar al perfil del usuario.2)Presionar botón "seguir".</t>
+  </si>
+  <si>
+    <t>Cambia a siguiendo</t>
+  </si>
+  <si>
+    <t>Dejar de seguir</t>
+  </si>
+  <si>
+    <t>Validar eliminación de seguimiento</t>
+  </si>
+  <si>
+    <t>1)Ingresar al perfil del usuario.2)Presionar botón "siguiendo".3) Opción dejar de seguir</t>
+  </si>
+  <si>
+    <t>Se elimina de la lista de seguidos</t>
+  </si>
+  <si>
+    <t>Seguir perfil privado</t>
+  </si>
+  <si>
+    <t>Validar solicitud perfil privado</t>
+  </si>
+  <si>
+    <t>No seguir previamente al usuario</t>
+  </si>
+  <si>
+    <t>Click en seguir</t>
+  </si>
+  <si>
+    <t>Muestra cartel de "Pendiente"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF212529"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -217,9 +712,27 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7E1CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="4">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -233,70 +746,111 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -304,7 +858,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -494,34 +1048,40 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="30.25"/>
-    <col customWidth="1" min="3" max="3" width="32.88"/>
-    <col customWidth="1" min="4" max="4" width="34.13"/>
-    <col customWidth="1" min="5" max="5" width="28.88"/>
-    <col customWidth="1" min="6" max="6" width="24.13"/>
-    <col customWidth="1" min="7" max="7" width="41.63"/>
-    <col customWidth="1" min="8" max="8" width="30.13"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="7" max="7" width="41.5703125" customWidth="1"/>
+    <col min="8" max="8" width="40.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1"/>
@@ -537,7 +1097,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -549,7 +1109,7 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1"/>
@@ -560,7 +1120,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -575,201 +1135,949 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="B5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="B6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="B7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="B8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="B9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="B10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="B11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="B13" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="B14" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="B15" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="B16" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="B17" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="B18" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="B19" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="s">
+      <c r="B20" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="B21" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="s">
+      <c r="B22" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="7" t="s">
+      <c r="B23" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="7" t="s">
+      <c r="B24" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="s">
+      <c r="B25" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="7" t="s">
+      <c r="B26" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="B27" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="s">
+      <c r="B28" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="7" t="s">
+      <c r="B29" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="7" t="s">
+      <c r="B30" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="7" t="s">
+      <c r="B31" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="I31" s="9"/>
+      <c r="J31" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="7" t="s">
+      <c r="B32" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="7" t="s">
+      <c r="B33" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="B34" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J1:J1000">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="J1:J4 J35:J1000">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1000">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1" display="http://qa_user31hotmail.com/" xr:uid="{B3D57A4D-418E-4C3B-B92E-4BA92B8963E9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modifico matriz de casos de pruebas
</commit_message>
<xml_diff>
--- a/casos_de_prueba/matriz_pruebas.xlsx
+++ b/casos_de_prueba/matriz_pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ProyectoFinal\ProyectoFinal-Nerea\casos_de_prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB83ED-4D5B-4FC7-B758-72D04BFB38B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F4F2A6-5004-4FA1-89C4-D36350F45D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="205">
   <si>
     <t>Nombre del Proyecto:</t>
   </si>
@@ -629,6 +629,12 @@
   </si>
   <si>
     <t>Muestra cartel de "Pendiente"</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Media</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1066,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1072,11 +1078,11 @@
     <col min="5" max="5" width="41.85546875" customWidth="1"/>
     <col min="6" max="6" width="50" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" customWidth="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1"/>
+    <col min="8" max="8" width="46.28515625" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1103,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1120,7 +1126,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1193,12 +1199,14 @@
       <c r="H5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>203</v>
+      </c>
       <c r="J5" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1223,12 +1231,14 @@
       <c r="H6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J6" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -1253,12 +1263,14 @@
       <c r="H7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J7" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1283,12 +1295,14 @@
       <c r="H8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J8" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
@@ -1313,12 +1327,14 @@
       <c r="H9" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J9" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -1343,12 +1359,14 @@
       <c r="H10" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J10" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -1373,12 +1391,14 @@
       <c r="H11" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J11" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
@@ -1403,12 +1423,14 @@
       <c r="H12" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J12" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -1433,12 +1455,14 @@
       <c r="H13" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J13" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
@@ -1463,12 +1487,14 @@
       <c r="H14" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J14" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
@@ -1493,12 +1519,14 @@
       <c r="H15" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J15" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
@@ -1523,12 +1551,14 @@
       <c r="H16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J16" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
@@ -1553,12 +1583,14 @@
       <c r="H17" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J17" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1583,7 +1615,9 @@
       <c r="H18" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J18" s="10" t="s">
         <v>53</v>
       </c>
@@ -1613,12 +1647,14 @@
       <c r="H19" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J19" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
@@ -1641,12 +1677,14 @@
       <c r="H20" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="I20" s="9"/>
+      <c r="I20" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J20" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
@@ -1671,12 +1709,14 @@
       <c r="H21" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J21" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
@@ -1701,12 +1741,14 @@
       <c r="H22" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J22" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
@@ -1731,12 +1773,14 @@
       <c r="H23" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J23" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
@@ -1761,12 +1805,14 @@
       <c r="H24" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J24" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
@@ -1791,7 +1837,9 @@
       <c r="H25" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J25" s="10" t="s">
         <v>53</v>
       </c>
@@ -1821,12 +1869,14 @@
       <c r="H26" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J26" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>39</v>
       </c>
@@ -1851,7 +1901,9 @@
       <c r="H27" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J27" s="10" t="s">
         <v>53</v>
       </c>
@@ -1881,12 +1933,14 @@
       <c r="H28" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J28" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>41</v>
       </c>
@@ -1911,12 +1965,14 @@
       <c r="H29" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J29" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>42</v>
       </c>
@@ -1941,12 +1997,14 @@
       <c r="H30" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J30" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>43</v>
       </c>
@@ -1971,12 +2029,14 @@
       <c r="H31" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="9" t="s">
+        <v>204</v>
+      </c>
       <c r="J31" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>44</v>
       </c>
@@ -2001,12 +2061,14 @@
       <c r="H32" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="I32" s="9"/>
+      <c r="I32" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J32" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
@@ -2031,7 +2093,9 @@
       <c r="H33" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="I33" s="9"/>
+      <c r="I33" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J33" s="10" t="s">
         <v>53</v>
       </c>
@@ -2061,7 +2125,9 @@
       <c r="H34" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="I34" s="9"/>
+      <c r="I34" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="J34" s="10" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Modifico casos de pruebas
</commit_message>
<xml_diff>
--- a/casos_de_prueba/matriz_pruebas.xlsx
+++ b/casos_de_prueba/matriz_pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ProyectoFinal\ProyectoFinal-Nerea\casos_de_prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F4F2A6-5004-4FA1-89C4-D36350F45D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE271EA2-CA29-4A96-9989-5AA1B0F1E5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,9 +283,6 @@
     <t>1)Completar email válido. 2)Siguiente3)completar codigo enviado por mail.4)completar nombre y contraseña SIN NÚMEROS</t>
   </si>
   <si>
-    <t>Muestra cartel de ¨La contraseña debe tener números¨</t>
-  </si>
-  <si>
     <t>El sistema permite contraseña y pasa a próximo paso</t>
   </si>
   <si>
@@ -635,6 +632,9 @@
   </si>
   <si>
     <t>Media</t>
+  </si>
+  <si>
+    <t>El sistema permite contraseña</t>
   </si>
 </sst>
 </file>
@@ -652,17 +652,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF212529"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -670,11 +673,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1066,8 +1071,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1200,7 +1205,7 @@
         <v>52</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>53</v>
@@ -1232,7 +1237,7 @@
         <v>59</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>53</v>
@@ -1264,7 +1269,7 @@
         <v>59</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>53</v>
@@ -1296,7 +1301,7 @@
         <v>69</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>53</v>
@@ -1328,7 +1333,7 @@
         <v>74</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>53</v>
@@ -1360,7 +1365,7 @@
         <v>59</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>53</v>
@@ -1392,7 +1397,7 @@
         <v>59</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>53</v>
@@ -1418,16 +1423,16 @@
         <v>86</v>
       </c>
       <c r="G12" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="I12" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>89</v>
+        <v>202</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -1435,28 +1440,28 @@
         <v>25</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="H13" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J13" s="10" t="s">
         <v>53</v>
@@ -1467,28 +1472,28 @@
         <v>26</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>100</v>
-      </c>
       <c r="H14" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>53</v>
@@ -1499,28 +1504,28 @@
         <v>27</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="H15" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>53</v>
@@ -1531,28 +1536,28 @@
         <v>28</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>59</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>53</v>
@@ -1563,28 +1568,28 @@
         <v>29</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>117</v>
-      </c>
       <c r="H17" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>53</v>
@@ -1595,28 +1600,28 @@
         <v>30</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="H18" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J18" s="10" t="s">
         <v>53</v>
@@ -1627,31 +1632,31 @@
         <v>31</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="I19" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -1659,29 +1664,29 @@
         <v>32</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>135</v>
-      </c>
       <c r="I20" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -1689,28 +1694,28 @@
         <v>33</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="H21" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>53</v>
@@ -1721,28 +1726,28 @@
         <v>34</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>143</v>
-      </c>
       <c r="H22" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>53</v>
@@ -1753,28 +1758,28 @@
         <v>35</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>148</v>
-      </c>
       <c r="H23" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J23" s="10" t="s">
         <v>53</v>
@@ -1785,31 +1790,31 @@
         <v>36</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="E24" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="I24" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1817,28 +1822,28 @@
         <v>37</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="I25" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J25" s="10" t="s">
         <v>53</v>
@@ -1849,28 +1854,28 @@
         <v>38</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="E26" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="G26" s="9" t="s">
+      <c r="H26" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>165</v>
-      </c>
       <c r="I26" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J26" s="10" t="s">
         <v>53</v>
@@ -1881,28 +1886,28 @@
         <v>39</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>169</v>
-      </c>
       <c r="H27" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J27" s="10" t="s">
         <v>53</v>
@@ -1913,28 +1918,28 @@
         <v>40</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>173</v>
-      </c>
       <c r="H28" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>53</v>
@@ -1945,28 +1950,28 @@
         <v>41</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="E29" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>178</v>
-      </c>
       <c r="H29" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>53</v>
@@ -1977,28 +1982,28 @@
         <v>42</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="E30" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>183</v>
-      </c>
       <c r="H30" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J30" s="10" t="s">
         <v>53</v>
@@ -2009,28 +2014,28 @@
         <v>43</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="E31" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>188</v>
-      </c>
       <c r="H31" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J31" s="10" t="s">
         <v>53</v>
@@ -2041,28 +2046,28 @@
         <v>44</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="D32" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="E32" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="9" t="s">
+      <c r="G32" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="H32" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J32" s="10" t="s">
         <v>53</v>
@@ -2073,28 +2078,28 @@
         <v>45</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="D33" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="9" t="s">
+      <c r="G33" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>197</v>
-      </c>
       <c r="H33" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>53</v>
@@ -2105,28 +2110,28 @@
         <v>46</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="D34" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="E34" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34" s="9" t="s">
+      <c r="G34" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="H34" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>203</v>
       </c>
       <c r="J34" s="10" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
modifico matriz de pruebas
</commit_message>
<xml_diff>
--- a/casos_de_prueba/matriz_pruebas.xlsx
+++ b/casos_de_prueba/matriz_pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ProyectoFinal\ProyectoFinal-Nerea\casos_de_prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE271EA2-CA29-4A96-9989-5AA1B0F1E5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6B1CF3-8704-4972-9E15-CD6E67A44CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1071,8 +1071,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>